<commit_message>
prune some dp calculation
</commit_message>
<xml_diff>
--- a/exp/results/exp3_url_ann_lbf.xlsx
+++ b/exp/results/exp3_url_ann_lbf.xlsx
@@ -1,118 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python\LBF-STK\exp\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFB9AA5-F10D-4E87-920B-2F4FD28B5ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>0.10707392113051718</t>
-  </si>
-  <si>
-    <t>0.39086134085139734</t>
-  </si>
-  <si>
-    <t>0.02807575775300352</t>
-  </si>
-  <si>
-    <t>0.09486096650796065</t>
-  </si>
-  <si>
-    <t>0.05319186270954459</t>
-  </si>
-  <si>
-    <t>0.028473497654504406</t>
-  </si>
-  <si>
-    <t>0.03723547371992092</t>
-  </si>
-  <si>
-    <t>0.035667910578711555</t>
-  </si>
-  <si>
-    <t>0.03596036638863868</t>
-  </si>
-  <si>
-    <t>0.03706000023396465</t>
-  </si>
-  <si>
-    <t>0.05279412280804371</t>
-  </si>
-  <si>
-    <t>0.06952259513587497</t>
-  </si>
-  <si>
-    <t>0.03997286010083876</t>
-  </si>
-  <si>
-    <t>0.033585625212030464</t>
-  </si>
-  <si>
-    <t>0.03321128177532375</t>
-  </si>
-  <si>
-    <t>0.03495431840248939</t>
-  </si>
-  <si>
-    <t>0.033959968648737175</t>
-  </si>
-  <si>
-    <t>0.037422645438274275</t>
-  </si>
-  <si>
-    <t>0.044347999017348476</t>
-  </si>
-  <si>
-    <t>0.033913175719148834</t>
-  </si>
-  <si>
-    <t>Our</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.0262508334990582</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -130,23 +46,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -434,185 +408,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" t="n">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0.3866148824912556</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.0694991986710808</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.03702490553677339</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.1130517178854275</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.03174900272568815</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.034591673198179754</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.047506521764561375</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>80</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.04046418586151632</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>90</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.03813623761449645</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>100</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.03138635752137852</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>110</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.03102371231706889</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>120</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.029374261549079933</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>130</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0.03815963407929062</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>140</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0.037200379022729664</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>150</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0.03173730449329106</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>160</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0.03198296737362984</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>170</v>
       </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.0342524244586643</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>180</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0.029982569633728345</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>190</v>
       </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.03159692570452605</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>200</v>
       </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0.035761496437888236</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>